<commit_message>
Agregar boleto de colectivo (falta testearlo)
</commit_message>
<xml_diff>
--- a/Documentacion/Casos de uso/Casos de uso.xlsx
+++ b/Documentacion/Casos de uso/Casos de uso.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{DE5B1A62-9786-4F4F-B69E-48E88DC62968}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5668CD24-17BB-40EF-BF63-8C5BC133D8B4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
   <si>
     <t>Nro</t>
   </si>
@@ -85,9 +85,6 @@
     <t>agregarBoleto</t>
   </si>
   <si>
-    <t>Agrega un boleto de colectivo</t>
-  </si>
-  <si>
     <t>AdminDeLectoras</t>
   </si>
   <si>
@@ -187,27 +184,9 @@
     <t>Carga la tarjeta haciendo uso del beneficio de boleto estudiantil.</t>
   </si>
   <si>
-    <t xml:space="preserve">boletos:List&lt;Boleto&gt;, montoBoletoActual: float, </t>
-  </si>
-  <si>
-    <t>montoRedSube: float</t>
-  </si>
-  <si>
-    <t>Revisa los viajes hechos en las ultimas 2 horas y calcula el monto del viaje actual.</t>
-  </si>
-  <si>
-    <t>devuelve el monto del viaje actual con el descuento de la tarifa Social.</t>
-  </si>
-  <si>
-    <t>montoBoletoActual: float</t>
-  </si>
-  <si>
     <t>montoTarifaSocial: float</t>
   </si>
   <si>
-    <t>CalculoDeBeneficios</t>
-  </si>
-  <si>
     <t>traerUsuario</t>
   </si>
   <si>
@@ -281,6 +260,39 @@
   </si>
   <si>
     <t>lectora: LectoraAutonoma</t>
+  </si>
+  <si>
+    <t>traerBoletosRedSube</t>
+  </si>
+  <si>
+    <t>MovimientoAlta</t>
+  </si>
+  <si>
+    <t>Crea un objeto boleto con tramo de colectivo y le resta el saldo a la tarjeta.</t>
+  </si>
+  <si>
+    <t>agrega un boleto a la base de datos</t>
+  </si>
+  <si>
+    <t>boleto:Boleto</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>traerTarifaSocial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boletos:List&lt;Boleto&gt;, nuevoBoleto: Boleto </t>
+  </si>
+  <si>
+    <t>Al nuevo boleto le cambia el monto (si corresponde) revisando los boletos de las ultimas 2 horas.</t>
+  </si>
+  <si>
+    <t>nuevoBoleto: Boleto</t>
+  </si>
+  <si>
+    <t>Al nuevo boleto le cambia el monto (si corresponde) descontando el porcentaje de la tarifa social.</t>
   </si>
 </sst>
 </file>
@@ -598,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,7 +621,7 @@
     <col min="1" max="1" width="7" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="80.42578125" customWidth="1"/>
+    <col min="4" max="4" width="95.85546875" customWidth="1"/>
     <col min="5" max="5" width="98.28515625" customWidth="1"/>
     <col min="6" max="6" width="27.140625" customWidth="1"/>
   </cols>
@@ -659,7 +671,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -693,7 +705,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -710,7 +722,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -721,7 +733,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -730,7 +742,7 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -741,19 +753,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,19 +773,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,19 +793,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -801,16 +813,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -818,16 +830,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -835,19 +847,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" t="s">
         <v>27</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -855,19 +867,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" t="s">
-        <v>31</v>
-      </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -875,16 +887,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -892,19 +904,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
         <v>36</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -912,16 +924,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -929,19 +941,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -949,19 +958,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="F19" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -969,19 +978,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>56</v>
+      </c>
+      <c r="F20" t="s">
         <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -989,19 +998,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1009,19 +1018,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1029,19 +1038,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
         <v>39</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1049,19 +1058,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F24" t="s">
         <v>39</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" t="s">
-        <v>48</v>
-      </c>
-      <c r="F24" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1069,19 +1078,58 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
         <v>39</v>
       </c>
-      <c r="C25" t="s">
-        <v>49</v>
-      </c>
-      <c r="D25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" t="s">
-        <v>40</v>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E26" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testeo de agregar boleto colectivo
La consulta de  traerTarjetaConBeneficios no anda, devuelve siempre null.
</commit_message>
<xml_diff>
--- a/Documentacion/Casos de uso/Casos de uso.xlsx
+++ b/Documentacion/Casos de uso/Casos de uso.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5668CD24-17BB-40EF-BF63-8C5BC133D8B4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{92FA3C94-A730-4DEF-85EE-F34858FD03C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
   <si>
     <t>Nro</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>Al nuevo boleto le cambia el monto (si corresponde) descontando el porcentaje de la tarifa social.</t>
+  </si>
+  <si>
+    <t>traerTarjetaConBeneficios</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,6 +1135,17 @@
         <v>86</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agregar boleto de tren y subte + correccion del calculo de red sube
Se testeo el agregar boleto de subte. Falta testear el agregar boleto de tren (usan el mismo metodo)
</commit_message>
<xml_diff>
--- a/Documentacion/Casos de uso/Casos de uso.xlsx
+++ b/Documentacion/Casos de uso/Casos de uso.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{92FA3C94-A730-4DEF-85EE-F34858FD03C6}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20BAA452-470B-476E-BB5E-B9FDB8407195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="94">
   <si>
     <t>Nro</t>
   </si>
@@ -106,196 +106,202 @@
     <t>tramo: TramoColectivo</t>
   </si>
   <si>
+    <t>Trae un tramo de tren o subte.</t>
+  </si>
+  <si>
+    <t>estacion1: Estacion, estacion2: Estacion</t>
+  </si>
+  <si>
+    <t>cargarTarjeta</t>
+  </si>
+  <si>
+    <t>Carga una tarjeta activa.</t>
+  </si>
+  <si>
+    <t>Agrega un boleto de tren o subte.</t>
+  </si>
+  <si>
+    <t>consultarSaldo</t>
+  </si>
+  <si>
+    <t>Consulta el saldo de una tarjeta</t>
+  </si>
+  <si>
+    <t>saldo: float</t>
+  </si>
+  <si>
+    <t>Reporte</t>
+  </si>
+  <si>
+    <t>boletos: List&lt;Boleto&gt;</t>
+  </si>
+  <si>
+    <t>viajesRealizados</t>
+  </si>
+  <si>
+    <t>Devuelve una lista de viajes realizados por tipo de transporte.</t>
+  </si>
+  <si>
+    <t>viajesRealizadosColectivo</t>
+  </si>
+  <si>
+    <t>Devuelve una lista de viajes realizados por linea de colectivo.</t>
+  </si>
+  <si>
+    <t>viajesRealizadosTren</t>
+  </si>
+  <si>
+    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaColectivo: String</t>
+  </si>
+  <si>
+    <t>Devuelve una lista de viajes realizados por linea de tren.</t>
+  </si>
+  <si>
+    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaTren: String</t>
+  </si>
+  <si>
+    <t>viajesRealizadosSubte</t>
+  </si>
+  <si>
+    <t>Devuelve una lista de viajes realizados por linea de subte.</t>
+  </si>
+  <si>
+    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaSubte: String</t>
+  </si>
+  <si>
+    <t>calcularTarifaSocial</t>
+  </si>
+  <si>
+    <t>cargaBoletoEstudiantil</t>
+  </si>
+  <si>
+    <t>Carga la tarjeta haciendo uso del beneficio de boleto estudiantil.</t>
+  </si>
+  <si>
+    <t>montoTarifaSocial: float</t>
+  </si>
+  <si>
+    <t>traerUsuario</t>
+  </si>
+  <si>
+    <t>dni: int</t>
+  </si>
+  <si>
+    <t>validarUsuario</t>
+  </si>
+  <si>
+    <t>dni: int, password: String</t>
+  </si>
+  <si>
+    <t>Trae un usuario por dni.</t>
+  </si>
+  <si>
+    <t>SesionUsuario</t>
+  </si>
+  <si>
+    <t>Actualiza la tarjeta modificada en la base de datos.</t>
+  </si>
+  <si>
+    <t>usuario: Usuario</t>
+  </si>
+  <si>
+    <t>calcularRedSube</t>
+  </si>
+  <si>
+    <t>numeroSerieTarjeta: int</t>
+  </si>
+  <si>
+    <t>numeroSerieLectora: int</t>
+  </si>
+  <si>
+    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar, tramo: TramoColectivo</t>
+  </si>
+  <si>
+    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar</t>
+  </si>
+  <si>
+    <t>kMin: float, kMax: float</t>
+  </si>
+  <si>
+    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar, monto: int</t>
+  </si>
+  <si>
+    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, tipoTransporte: TipoTransporte</t>
+  </si>
+  <si>
+    <t>tipoUsuario: TipoUsuario</t>
+  </si>
+  <si>
+    <t>Valida la existencia del usuario y si la contraseña es correcta. Devuelve el tipo de usuario.</t>
+  </si>
+  <si>
+    <t>traerLectoraCarga</t>
+  </si>
+  <si>
+    <t>Trae una lectora de carga.</t>
+  </si>
+  <si>
+    <t>lectora: LectoraCarga</t>
+  </si>
+  <si>
+    <t>traerLectoraAutonoma</t>
+  </si>
+  <si>
+    <t>Trae una lectora autonoma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> numeroSerieLectora: int</t>
+  </si>
+  <si>
+    <t>lectora: LectoraAutonoma</t>
+  </si>
+  <si>
+    <t>traerBoletosRedSube</t>
+  </si>
+  <si>
+    <t>MovimientoAlta</t>
+  </si>
+  <si>
+    <t>Crea un objeto boleto con tramo de colectivo y le resta el saldo a la tarjeta.</t>
+  </si>
+  <si>
+    <t>agrega un boleto a la base de datos</t>
+  </si>
+  <si>
+    <t>boleto:Boleto</t>
+  </si>
+  <si>
+    <t>Funciones</t>
+  </si>
+  <si>
+    <t>traerTarifaSocial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boletos:List&lt;Boleto&gt;, nuevoBoleto: Boleto </t>
+  </si>
+  <si>
+    <t>Al nuevo boleto le cambia el monto (si corresponde) revisando los boletos de las ultimas 2 horas.</t>
+  </si>
+  <si>
+    <t>nuevoBoleto: Boleto</t>
+  </si>
+  <si>
+    <t>Al nuevo boleto le cambia el monto (si corresponde) descontando el porcentaje de la tarifa social.</t>
+  </si>
+  <si>
+    <t>traerTarjetaConBeneficios</t>
+  </si>
+  <si>
+    <t>TramosConsultas</t>
+  </si>
+  <si>
+    <t>traerUltimoBoleto</t>
+  </si>
+  <si>
     <t>traerTramoTrenYSubte</t>
   </si>
   <si>
-    <t>Trae un tramo de tren o subte.</t>
-  </si>
-  <si>
-    <t>estacion1: Estacion, estacion2: Estacion</t>
-  </si>
-  <si>
-    <t>cargarTarjeta</t>
-  </si>
-  <si>
-    <t>Carga una tarjeta activa.</t>
-  </si>
-  <si>
-    <t>TramosAdmin</t>
-  </si>
-  <si>
-    <t>Agrega un boleto de tren o subte.</t>
-  </si>
-  <si>
-    <t>consultarSaldo</t>
-  </si>
-  <si>
-    <t>Consulta el saldo de una tarjeta</t>
-  </si>
-  <si>
-    <t>saldo: float</t>
-  </si>
-  <si>
-    <t>Reporte</t>
-  </si>
-  <si>
-    <t>boletos: List&lt;Boleto&gt;</t>
-  </si>
-  <si>
-    <t>viajesRealizados</t>
-  </si>
-  <si>
-    <t>Devuelve una lista de viajes realizados por tipo de transporte.</t>
-  </si>
-  <si>
-    <t>viajesRealizadosColectivo</t>
-  </si>
-  <si>
-    <t>Devuelve una lista de viajes realizados por linea de colectivo.</t>
-  </si>
-  <si>
-    <t>viajesRealizadosTren</t>
-  </si>
-  <si>
-    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaColectivo: String</t>
-  </si>
-  <si>
-    <t>Devuelve una lista de viajes realizados por linea de tren.</t>
-  </si>
-  <si>
-    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaTren: String</t>
-  </si>
-  <si>
-    <t>viajesRealizadosSubte</t>
-  </si>
-  <si>
-    <t>Devuelve una lista de viajes realizados por linea de subte.</t>
-  </si>
-  <si>
-    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, lineaSubte: String</t>
-  </si>
-  <si>
-    <t>calcularTarifaSocial</t>
-  </si>
-  <si>
-    <t>cargaBoletoEstudiantil</t>
-  </si>
-  <si>
-    <t>Carga la tarjeta haciendo uso del beneficio de boleto estudiantil.</t>
-  </si>
-  <si>
-    <t>montoTarifaSocial: float</t>
-  </si>
-  <si>
-    <t>traerUsuario</t>
-  </si>
-  <si>
-    <t>dni: int</t>
-  </si>
-  <si>
-    <t>validarUsuario</t>
-  </si>
-  <si>
-    <t>dni: int, password: String</t>
-  </si>
-  <si>
-    <t>Trae un usuario por dni.</t>
-  </si>
-  <si>
-    <t>SesionUsuario</t>
-  </si>
-  <si>
-    <t>Actualiza la tarjeta modificada en la base de datos.</t>
-  </si>
-  <si>
-    <t>usuario: Usuario</t>
-  </si>
-  <si>
-    <t>calcularRedSube</t>
-  </si>
-  <si>
-    <t>numeroSerieTarjeta: int</t>
-  </si>
-  <si>
-    <t>numeroSerieLectora: int</t>
-  </si>
-  <si>
-    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar, tramo: TramoColectivo</t>
-  </si>
-  <si>
-    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar</t>
-  </si>
-  <si>
-    <t>kMin: float, kMax: float</t>
-  </si>
-  <si>
-    <t>numeroSerieLectora: int, tarjeta:Tarjeta, fechaHora: GregorianCalendar, monto: int</t>
-  </si>
-  <si>
-    <t>fechaDesde: GregorianCalendar, fechaHasta: GregorianCalendar, tipoTransporte: TipoTransporte</t>
-  </si>
-  <si>
-    <t>tipoUsuario: TipoUsuario</t>
-  </si>
-  <si>
-    <t>Valida la existencia del usuario y si la contraseña es correcta. Devuelve el tipo de usuario.</t>
-  </si>
-  <si>
-    <t>traerLectoraCarga</t>
-  </si>
-  <si>
-    <t>Trae una lectora de carga.</t>
-  </si>
-  <si>
-    <t>lectora: LectoraCarga</t>
-  </si>
-  <si>
-    <t>traerLectoraAutonoma</t>
-  </si>
-  <si>
-    <t>Trae una lectora autonoma.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> numeroSerieLectora: int</t>
-  </si>
-  <si>
-    <t>lectora: LectoraAutonoma</t>
-  </si>
-  <si>
-    <t>traerBoletosRedSube</t>
-  </si>
-  <si>
-    <t>MovimientoAlta</t>
-  </si>
-  <si>
-    <t>Crea un objeto boleto con tramo de colectivo y le resta el saldo a la tarjeta.</t>
-  </si>
-  <si>
-    <t>agrega un boleto a la base de datos</t>
-  </si>
-  <si>
-    <t>boleto:Boleto</t>
-  </si>
-  <si>
-    <t>Funciones</t>
-  </si>
-  <si>
-    <t>traerTarifaSocial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boletos:List&lt;Boleto&gt;, nuevoBoleto: Boleto </t>
-  </si>
-  <si>
-    <t>Al nuevo boleto le cambia el monto (si corresponde) revisando los boletos de las ultimas 2 horas.</t>
-  </si>
-  <si>
-    <t>nuevoBoleto: Boleto</t>
-  </si>
-  <si>
-    <t>Al nuevo boleto le cambia el monto (si corresponde) descontando el porcentaje de la tarifa social.</t>
-  </si>
-  <si>
-    <t>traerTarjetaConBeneficios</t>
+    <t>traerTramoUnaEstacion</t>
   </si>
 </sst>
 </file>
@@ -613,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +680,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
         <v>16</v>
@@ -708,7 +714,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -725,7 +731,7 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
@@ -745,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F7" t="s">
         <v>19</v>
@@ -765,7 +771,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>25</v>
@@ -779,16 +785,16 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" t="s">
         <v>73</v>
-      </c>
-      <c r="D9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E9" t="s">
-        <v>78</v>
-      </c>
-      <c r="F9" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,16 +805,16 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" t="s">
         <v>77</v>
-      </c>
-      <c r="E10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,10 +828,10 @@
         <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,10 +845,10 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,7 +856,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -859,7 +865,7 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F13" t="s">
         <v>27</v>
@@ -870,16 +876,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
       </c>
       <c r="F14" t="s">
         <v>27</v>
@@ -893,13 +899,13 @@
         <v>21</v>
       </c>
       <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
         <v>31</v>
       </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -910,16 +916,16 @@
         <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,13 +936,13 @@
         <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -944,16 +950,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
         <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,19 +967,19 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,19 +987,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,19 +1007,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1021,19 +1027,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
         <v>38</v>
       </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E22" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,19 +1047,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
         <v>43</v>
       </c>
-      <c r="E23" t="s">
-        <v>45</v>
-      </c>
       <c r="F23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,19 +1067,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s">
         <v>44</v>
       </c>
-      <c r="D24" t="s">
-        <v>46</v>
-      </c>
       <c r="E24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,19 +1087,19 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" t="s">
         <v>48</v>
       </c>
-      <c r="D25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" t="s">
-        <v>50</v>
-      </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,16 +1107,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
         <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1118,10 +1124,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1132,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1143,6 +1149,19 @@
         <v>6</v>
       </c>
       <c r="C29" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregar boleto de tren y subte (no esta funcionando)
No funciona porque no los metodos traerTramoUnaEstacion y traerTramoTrenYSubte devuelven null. Estan todos los tests armados y algunos tienen codigo comentado que sirve para agregar lo que sea necesario (estaciones, lectoras, etc).
</commit_message>
<xml_diff>
--- a/Documentacion/Casos de uso/Casos de uso.xlsx
+++ b/Documentacion/Casos de uso/Casos de uso.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20BAA452-470B-476E-BB5E-B9FDB8407195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54EFCD67-BB60-464C-BC89-26CEFE33F72D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
   <si>
     <t>Nro</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>traerTramoUnaEstacion</t>
+  </si>
+  <si>
+    <t>traerTransportePorTipo</t>
   </si>
 </sst>
 </file>
@@ -1160,6 +1163,11 @@
         <v>93</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
Traeme las Listas Cami.... Traeme las Lis
HACELOOOOOO
</commit_message>
<xml_diff>
--- a/Documentacion/Casos de uso/Casos de uso.xlsx
+++ b/Documentacion/Casos de uso/Casos de uso.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54EFCD67-BB60-464C-BC89-26CEFE33F72D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{20BAA452-470B-476E-BB5E-B9FDB8407195}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="94">
   <si>
     <t>Nro</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>traerTramoUnaEstacion</t>
-  </si>
-  <si>
-    <t>traerTransportePorTipo</t>
   </si>
 </sst>
 </file>
@@ -1163,11 +1160,6 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>91</v>

</xml_diff>